<commit_message>
updated sprites + placeholders for raging bolt iron crown
</commit_message>
<xml_diff>
--- a/pokemon_species_names_bp.xlsx
+++ b/pokemon_species_names_bp.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$M$1:$Q$1155</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$M$1:$Q$1157</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9129" uniqueCount="6434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9162" uniqueCount="6455">
   <si>
     <t>Bulbasaur</t>
   </si>
@@ -19329,6 +19329,69 @@
   </si>
   <si>
     <t>テラパゴス</t>
+  </si>
+  <si>
+    <t>Iron Crown</t>
+  </si>
+  <si>
+    <t>Raging Bolt</t>
+  </si>
+  <si>
+    <t>Furienblitz</t>
+  </si>
+  <si>
+    <t>Eisenhaupt</t>
+  </si>
+  <si>
+    <t>Chef-de-Fer</t>
+  </si>
+  <si>
+    <t>Ire-Foudre</t>
+  </si>
+  <si>
+    <t>タケルライコ</t>
+  </si>
+  <si>
+    <t>날뛰는우레</t>
+  </si>
+  <si>
+    <t>猛雷鼓</t>
+  </si>
+  <si>
+    <t>Ferrotesta</t>
+  </si>
+  <si>
+    <t>Capoferreo</t>
+  </si>
+  <si>
+    <t>テツノカシラ</t>
+  </si>
+  <si>
+    <t>무쇠감투</t>
+  </si>
+  <si>
+    <t>鐵頭殼</t>
+  </si>
+  <si>
+    <t>Electrofuria</t>
+  </si>
+  <si>
+    <t>Furiatonante</t>
+  </si>
+  <si>
+    <t>오거폰</t>
+  </si>
+  <si>
+    <t>테라파고스</t>
+  </si>
+  <si>
+    <t>기로치</t>
+  </si>
+  <si>
+    <t>조타구</t>
+  </si>
+  <si>
+    <t>이야후</t>
   </si>
 </sst>
 </file>
@@ -19647,10 +19710,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1017"/>
+  <dimension ref="A1:J1019"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A294" workbookViewId="0">
-      <selection activeCell="I264" sqref="I264"/>
+    <sheetView tabSelected="1" topLeftCell="A990" workbookViewId="0">
+      <selection activeCell="E1022" sqref="E1022"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -52017,103 +52080,212 @@
         <v>6407</v>
       </c>
     </row>
+    <row r="1012" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1012">
+        <v>1011</v>
+      </c>
+      <c r="B1012" t="s">
+        <v>6435</v>
+      </c>
+      <c r="C1012" t="s">
+        <v>6439</v>
+      </c>
+      <c r="D1012" t="s">
+        <v>6436</v>
+      </c>
+      <c r="E1012" t="s">
+        <v>6441</v>
+      </c>
+      <c r="F1012" t="s">
+        <v>6440</v>
+      </c>
+      <c r="G1012" t="s">
+        <v>6448</v>
+      </c>
+      <c r="H1012" t="s">
+        <v>6449</v>
+      </c>
+      <c r="I1012" t="s">
+        <v>6442</v>
+      </c>
+      <c r="J1012" t="s">
+        <v>6442</v>
+      </c>
+    </row>
     <row r="1013" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1013">
+        <v>1012</v>
+      </c>
       <c r="B1013" t="s">
-        <v>6408</v>
+        <v>6434</v>
       </c>
       <c r="C1013" t="s">
-        <v>6408</v>
+        <v>6438</v>
       </c>
       <c r="D1013" t="s">
-        <v>6408</v>
+        <v>6437</v>
+      </c>
+      <c r="E1013" t="s">
+        <v>6446</v>
       </c>
       <c r="F1013" t="s">
-        <v>6429</v>
+        <v>6445</v>
+      </c>
+      <c r="G1013" t="s">
+        <v>6443</v>
+      </c>
+      <c r="H1013" t="s">
+        <v>6444</v>
       </c>
       <c r="I1013" t="s">
-        <v>6409</v>
+        <v>6447</v>
       </c>
       <c r="J1013" t="s">
-        <v>6410</v>
-      </c>
-    </row>
-    <row r="1014" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B1014" t="s">
-        <v>6411</v>
-      </c>
-      <c r="C1014" t="s">
-        <v>6423</v>
-      </c>
-      <c r="D1014" t="s">
-        <v>6426</v>
-      </c>
-      <c r="F1014" t="s">
-        <v>6430</v>
-      </c>
-      <c r="I1014" t="s">
-        <v>6412</v>
-      </c>
-      <c r="J1014" t="s">
-        <v>6413</v>
+        <v>6447</v>
       </c>
     </row>
     <row r="1015" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1015" t="s">
-        <v>6414</v>
+        <v>6408</v>
       </c>
       <c r="C1015" t="s">
-        <v>6424</v>
+        <v>6408</v>
       </c>
       <c r="D1015" t="s">
-        <v>6427</v>
+        <v>6408</v>
+      </c>
+      <c r="E1015" t="s">
+        <v>6450</v>
       </c>
       <c r="F1015" t="s">
-        <v>6431</v>
+        <v>6429</v>
+      </c>
+      <c r="G1015" t="s">
+        <v>6408</v>
+      </c>
+      <c r="H1015" t="s">
+        <v>6408</v>
       </c>
       <c r="I1015" t="s">
-        <v>6415</v>
+        <v>6409</v>
       </c>
       <c r="J1015" t="s">
-        <v>6416</v>
+        <v>6410</v>
       </c>
     </row>
     <row r="1016" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1016" t="s">
-        <v>6417</v>
+        <v>6411</v>
       </c>
       <c r="C1016" t="s">
-        <v>6425</v>
+        <v>6423</v>
       </c>
       <c r="D1016" t="s">
-        <v>6428</v>
+        <v>6426</v>
+      </c>
+      <c r="E1016" t="s">
+        <v>6453</v>
       </c>
       <c r="F1016" t="s">
-        <v>6432</v>
+        <v>6430</v>
+      </c>
+      <c r="G1016" t="s">
+        <v>6411</v>
+      </c>
+      <c r="H1016" t="s">
+        <v>6411</v>
       </c>
       <c r="I1016" t="s">
-        <v>6418</v>
+        <v>6412</v>
       </c>
       <c r="J1016" t="s">
-        <v>6419</v>
+        <v>6413</v>
       </c>
     </row>
     <row r="1017" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1017" t="s">
+        <v>6414</v>
+      </c>
+      <c r="C1017" t="s">
+        <v>6424</v>
+      </c>
+      <c r="D1017" t="s">
+        <v>6427</v>
+      </c>
+      <c r="E1017" t="s">
+        <v>6454</v>
+      </c>
+      <c r="F1017" t="s">
+        <v>6431</v>
+      </c>
+      <c r="G1017" t="s">
+        <v>6414</v>
+      </c>
+      <c r="H1017" t="s">
+        <v>6414</v>
+      </c>
+      <c r="I1017" t="s">
+        <v>6415</v>
+      </c>
+      <c r="J1017" t="s">
+        <v>6416</v>
+      </c>
+    </row>
+    <row r="1018" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1018" t="s">
+        <v>6417</v>
+      </c>
+      <c r="C1018" t="s">
+        <v>6425</v>
+      </c>
+      <c r="D1018" t="s">
+        <v>6428</v>
+      </c>
+      <c r="E1018" t="s">
+        <v>6452</v>
+      </c>
+      <c r="F1018" t="s">
+        <v>6432</v>
+      </c>
+      <c r="G1018" t="s">
+        <v>6417</v>
+      </c>
+      <c r="H1018" t="s">
+        <v>6417</v>
+      </c>
+      <c r="I1018" t="s">
+        <v>6418</v>
+      </c>
+      <c r="J1018" t="s">
+        <v>6419</v>
+      </c>
+    </row>
+    <row r="1019" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1019" t="s">
         <v>6420</v>
       </c>
-      <c r="C1017" t="s">
+      <c r="C1019" t="s">
         <v>6420</v>
       </c>
-      <c r="D1017" t="s">
+      <c r="D1019" t="s">
         <v>6420</v>
       </c>
-      <c r="F1017" t="s">
+      <c r="E1019" t="s">
+        <v>6451</v>
+      </c>
+      <c r="F1019" t="s">
         <v>6433</v>
       </c>
-      <c r="I1017" t="s">
+      <c r="G1019" t="s">
+        <v>6420</v>
+      </c>
+      <c r="H1019" t="s">
+        <v>6420</v>
+      </c>
+      <c r="I1019" t="s">
         <v>6421</v>
       </c>
-      <c r="J1017" t="s">
+      <c r="J1019" t="s">
         <v>6422</v>
       </c>
     </row>

</xml_diff>

<commit_message>
iron crown raging bolt sprites updated
</commit_message>
<xml_diff>
--- a/pokemon_species_names_bp.xlsx
+++ b/pokemon_species_names_bp.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$M$1:$Q$1157</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$M$1:$Q$1160</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9162" uniqueCount="6455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9187" uniqueCount="6473">
   <si>
     <t>Bulbasaur</t>
   </si>
@@ -19392,6 +19392,60 @@
   </si>
   <si>
     <t>이야후</t>
+  </si>
+  <si>
+    <t>Dipplin</t>
+  </si>
+  <si>
+    <t>Archaludon</t>
+  </si>
+  <si>
+    <t>Poltchageist</t>
+  </si>
+  <si>
+    <t>カミッチュ</t>
+  </si>
+  <si>
+    <t>Pomdramour</t>
+  </si>
+  <si>
+    <t>Sirapfel</t>
+  </si>
+  <si>
+    <t>과미르</t>
+  </si>
+  <si>
+    <t>裹蜜蟲</t>
+  </si>
+  <si>
+    <t>裹蜜虫</t>
+  </si>
+  <si>
+    <t>ブリジュラス</t>
+  </si>
+  <si>
+    <t>Pondralugon</t>
+  </si>
+  <si>
+    <t>Briduradon</t>
+  </si>
+  <si>
+    <t>브리두라스</t>
+  </si>
+  <si>
+    <t>鋁鋼橋龍</t>
+  </si>
+  <si>
+    <t>铝钢桥龙</t>
+  </si>
+  <si>
+    <t>차데스</t>
+  </si>
+  <si>
+    <t>Mortcha</t>
+  </si>
+  <si>
+    <t>斯魔茶</t>
   </si>
 </sst>
 </file>
@@ -19710,10 +19764,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1019"/>
+  <dimension ref="A1:J1022"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A990" workbookViewId="0">
-      <selection activeCell="E1022" sqref="E1022"/>
+      <selection activeCell="K1005" sqref="K1005"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -52146,146 +52200,227 @@
     </row>
     <row r="1015" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1015" t="s">
-        <v>6408</v>
+        <v>6455</v>
       </c>
       <c r="C1015" t="s">
-        <v>6408</v>
+        <v>6459</v>
       </c>
       <c r="D1015" t="s">
-        <v>6408</v>
+        <v>6460</v>
       </c>
       <c r="E1015" t="s">
-        <v>6450</v>
+        <v>6461</v>
       </c>
       <c r="F1015" t="s">
-        <v>6429</v>
+        <v>6458</v>
       </c>
       <c r="G1015" t="s">
-        <v>6408</v>
+        <v>6455</v>
       </c>
       <c r="H1015" t="s">
-        <v>6408</v>
+        <v>6455</v>
       </c>
       <c r="I1015" t="s">
-        <v>6409</v>
+        <v>6462</v>
       </c>
       <c r="J1015" t="s">
-        <v>6410</v>
+        <v>6463</v>
       </c>
     </row>
     <row r="1016" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1016" t="s">
-        <v>6411</v>
+        <v>6456</v>
       </c>
       <c r="C1016" t="s">
-        <v>6423</v>
+        <v>6465</v>
       </c>
       <c r="D1016" t="s">
-        <v>6426</v>
+        <v>6466</v>
       </c>
       <c r="E1016" t="s">
-        <v>6453</v>
+        <v>6467</v>
       </c>
       <c r="F1016" t="s">
-        <v>6430</v>
+        <v>6464</v>
       </c>
       <c r="G1016" t="s">
-        <v>6411</v>
+        <v>6456</v>
       </c>
       <c r="H1016" t="s">
-        <v>6411</v>
+        <v>6456</v>
       </c>
       <c r="I1016" t="s">
-        <v>6412</v>
+        <v>6468</v>
       </c>
       <c r="J1016" t="s">
-        <v>6413</v>
+        <v>6469</v>
       </c>
     </row>
     <row r="1017" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1017" t="s">
-        <v>6414</v>
+        <v>6457</v>
       </c>
       <c r="C1017" t="s">
-        <v>6424</v>
+        <v>6457</v>
       </c>
       <c r="D1017" t="s">
-        <v>6427</v>
+        <v>6471</v>
       </c>
       <c r="E1017" t="s">
-        <v>6454</v>
-      </c>
-      <c r="F1017" t="s">
-        <v>6431</v>
+        <v>6470</v>
       </c>
       <c r="G1017" t="s">
-        <v>6414</v>
+        <v>6457</v>
       </c>
       <c r="H1017" t="s">
-        <v>6414</v>
+        <v>6457</v>
       </c>
       <c r="I1017" t="s">
-        <v>6415</v>
-      </c>
-      <c r="J1017" t="s">
-        <v>6416</v>
+        <v>6472</v>
       </c>
     </row>
     <row r="1018" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1018" t="s">
-        <v>6417</v>
+        <v>6408</v>
       </c>
       <c r="C1018" t="s">
-        <v>6425</v>
+        <v>6408</v>
       </c>
       <c r="D1018" t="s">
-        <v>6428</v>
+        <v>6408</v>
       </c>
       <c r="E1018" t="s">
-        <v>6452</v>
+        <v>6450</v>
       </c>
       <c r="F1018" t="s">
-        <v>6432</v>
+        <v>6429</v>
       </c>
       <c r="G1018" t="s">
-        <v>6417</v>
+        <v>6408</v>
       </c>
       <c r="H1018" t="s">
-        <v>6417</v>
+        <v>6408</v>
       </c>
       <c r="I1018" t="s">
-        <v>6418</v>
+        <v>6409</v>
       </c>
       <c r="J1018" t="s">
-        <v>6419</v>
+        <v>6410</v>
       </c>
     </row>
     <row r="1019" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1019" t="s">
+        <v>6411</v>
+      </c>
+      <c r="C1019" t="s">
+        <v>6423</v>
+      </c>
+      <c r="D1019" t="s">
+        <v>6426</v>
+      </c>
+      <c r="E1019" t="s">
+        <v>6453</v>
+      </c>
+      <c r="F1019" t="s">
+        <v>6430</v>
+      </c>
+      <c r="G1019" t="s">
+        <v>6411</v>
+      </c>
+      <c r="H1019" t="s">
+        <v>6411</v>
+      </c>
+      <c r="I1019" t="s">
+        <v>6412</v>
+      </c>
+      <c r="J1019" t="s">
+        <v>6413</v>
+      </c>
+    </row>
+    <row r="1020" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1020" t="s">
+        <v>6414</v>
+      </c>
+      <c r="C1020" t="s">
+        <v>6424</v>
+      </c>
+      <c r="D1020" t="s">
+        <v>6427</v>
+      </c>
+      <c r="E1020" t="s">
+        <v>6454</v>
+      </c>
+      <c r="F1020" t="s">
+        <v>6431</v>
+      </c>
+      <c r="G1020" t="s">
+        <v>6414</v>
+      </c>
+      <c r="H1020" t="s">
+        <v>6414</v>
+      </c>
+      <c r="I1020" t="s">
+        <v>6415</v>
+      </c>
+      <c r="J1020" t="s">
+        <v>6416</v>
+      </c>
+    </row>
+    <row r="1021" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1021" t="s">
+        <v>6417</v>
+      </c>
+      <c r="C1021" t="s">
+        <v>6425</v>
+      </c>
+      <c r="D1021" t="s">
+        <v>6428</v>
+      </c>
+      <c r="E1021" t="s">
+        <v>6452</v>
+      </c>
+      <c r="F1021" t="s">
+        <v>6432</v>
+      </c>
+      <c r="G1021" t="s">
+        <v>6417</v>
+      </c>
+      <c r="H1021" t="s">
+        <v>6417</v>
+      </c>
+      <c r="I1021" t="s">
+        <v>6418</v>
+      </c>
+      <c r="J1021" t="s">
+        <v>6419</v>
+      </c>
+    </row>
+    <row r="1022" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1022" t="s">
         <v>6420</v>
       </c>
-      <c r="C1019" t="s">
+      <c r="C1022" t="s">
         <v>6420</v>
       </c>
-      <c r="D1019" t="s">
+      <c r="D1022" t="s">
         <v>6420</v>
       </c>
-      <c r="E1019" t="s">
+      <c r="E1022" t="s">
         <v>6451</v>
       </c>
-      <c r="F1019" t="s">
+      <c r="F1022" t="s">
         <v>6433</v>
       </c>
-      <c r="G1019" t="s">
+      <c r="G1022" t="s">
         <v>6420</v>
       </c>
-      <c r="H1019" t="s">
+      <c r="H1022" t="s">
         <v>6420</v>
       </c>
-      <c r="I1019" t="s">
+      <c r="I1022" t="s">
         <v>6421</v>
       </c>
-      <c r="J1019" t="s">
+      <c r="J1022" t="s">
         <v>6422</v>
       </c>
     </row>

</xml_diff>